<commit_message>
Configuración de cargue de usuarios realizada
</commit_message>
<xml_diff>
--- a/public/users.xlsx
+++ b/public/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13d2ad5f67de6611/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{32C85B41-6F1F-4D77-B66A-768EEE2B442E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A3237B9-F91D-469F-B9DC-5F8EBB2A0698}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{32C85B41-6F1F-4D77-B66A-768EEE2B442E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8794FF94-8565-4E90-B2AA-A5AB16F6C38D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C6824096-AEFD-469D-B539-553F09206511}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -74,13 +74,55 @@
     <t>calle siempreviva 123</t>
   </si>
   <si>
-    <t>testeusertest2</t>
-  </si>
-  <si>
-    <t>ttestteo2</t>
-  </si>
-  <si>
     <t>https://www.google.com/url?sa=i&amp;url=https%3A%2F%2Fes.123rf.com%2Fphoto_59070200_icono-de-usuario-hombre-perfil-hombre-de-negocios-avatar-icono-persona-en-la-ilustraci%25C3%25B3n-vectorial.html&amp;psig=AOvVaw0KE_280JdOEhHeKpuGBrjB&amp;ust=1645566286766000&amp;source=images&amp;cd=vfe&amp;ved=0CAsQjRxqFwoTCIizhqPikfYCFQAAAAAdAAAAABAD</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>ttestteo4</t>
+  </si>
+  <si>
+    <t>ttestteo5</t>
+  </si>
+  <si>
+    <t>ttestteo6</t>
+  </si>
+  <si>
+    <t>ttestteo7</t>
+  </si>
+  <si>
+    <t>ttestteo8</t>
+  </si>
+  <si>
+    <t>ttestteo9</t>
+  </si>
+  <si>
+    <t>ttestteo10</t>
+  </si>
+  <si>
+    <t>testeusertest4</t>
+  </si>
+  <si>
+    <t>testeusertest5</t>
+  </si>
+  <si>
+    <t>testeusertest6</t>
+  </si>
+  <si>
+    <t>testeusertest7</t>
+  </si>
+  <si>
+    <t>testeusertest8</t>
+  </si>
+  <si>
+    <t>testeusertest9</t>
+  </si>
+  <si>
+    <t>testeusertest10</t>
+  </si>
+  <si>
+    <t>Estudiante</t>
   </si>
 </sst>
 </file>
@@ -452,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FB0E3E-2C2F-402E-BA09-77ABE181763B}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +539,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -506,32 +548,230 @@
         <v>123456</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2">
-        <v>3</v>
+      <c r="F2" t="s">
+        <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2">
         <v>3007819686</v>
       </c>
       <c r="J2">
+        <v>12345679987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>123456</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3">
+        <v>3007819686</v>
+      </c>
+      <c r="J3">
+        <v>12345679987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>123456</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>3007819686</v>
+      </c>
+      <c r="J4">
+        <v>12345679987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>123456</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5">
+        <v>3007819686</v>
+      </c>
+      <c r="J5">
+        <v>12345679987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>123456</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6">
+        <v>3007819686</v>
+      </c>
+      <c r="J6">
+        <v>12345679987</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>123456</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7">
+        <v>3007819686</v>
+      </c>
+      <c r="J7">
+        <v>12345679987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>123456</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>3007819686</v>
+      </c>
+      <c r="J8">
         <v>12345679987</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{7A8DF7F1-8B1C-4DCD-8929-9F17B0E62CE6}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{5BCD9E98-A0D3-42DB-8D3A-F403ECA1A135}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{25FC3F1A-0BD8-4E93-96F7-AB9BC60523CF}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{2D267AA8-0052-48D7-AFBD-E9B3B0AA4075}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{C79E1854-93FF-43AA-BDD0-A4C98174890A}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{5136F24A-F92B-4977-891E-64BCB1693FC6}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{2B9488D1-0FDF-4533-82DD-0B0721B336C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Configuracion incompleta de studentsClassroomImport, pendiente lectura de datos
</commit_message>
<xml_diff>
--- a/public/users.xlsx
+++ b/public/users.xlsx
@@ -8,47 +8,69 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13d2ad5f67de6611/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{7B87B841-B9C0-48B5-8F93-F35B0344CD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD6009FC-ECAE-483C-9D2B-DDDE87BFB62B}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{991C7F3C-61BB-4DDE-9A57-51A723AB719B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B21F83F-02C8-40C1-BDAA-F4756289D9FC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{116BEB94-D90C-4C81-877E-A94C4F0C1FC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C1531AC2-F34C-450B-B138-45E9EAA5FB07}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>classroom</t>
   </si>
   <si>
-    <t>user_name</t>
-  </si>
-  <si>
-    <t>testeusertest1</t>
+    <t>testk</t>
+  </si>
+  <si>
+    <t>prueba700</t>
+  </si>
+  <si>
+    <t>bukotujaby</t>
+  </si>
+  <si>
+    <t>hamaw</t>
+  </si>
+  <si>
+    <t>trikele_deiry</t>
+  </si>
+  <si>
+    <t>trikele_miguel</t>
+  </si>
+  <si>
+    <t>trikele_edgar</t>
+  </si>
+  <si>
+    <t>trikele_evelyn</t>
+  </si>
+  <si>
+    <t>trikele_matematicas</t>
+  </si>
+  <si>
+    <t>trikele_carolina</t>
+  </si>
+  <si>
+    <t>trikele_marlly</t>
+  </si>
+  <si>
+    <t>user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,13 +78,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,8 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,30 +430,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF234E4-22F0-4E77-8416-971629B41669}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99F327A-920D-4098-AFF7-B76F1AAC16A2}">
+  <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>